<commit_message>
Added excelReader, test data, rest assured utils
</commit_message>
<xml_diff>
--- a/src/test/resources/com/restapi/addplace/testdata/TestData - Copy.xlsx
+++ b/src/test/resources/com/restapi/addplace/testdata/TestData - Copy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>S.No.</t>
   </si>
@@ -36,10 +36,79 @@
     <t>qaclick123</t>
   </si>
   <si>
-    <t>contentType</t>
-  </si>
-  <si>
     <t>JSON</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>types</t>
+  </si>
+  <si>
+    <t>-38.383494</t>
+  </si>
+  <si>
+    <t>33.427362</t>
+  </si>
+  <si>
+    <t>Frontline house</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>pranjal.com</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Shop#Shoe Park</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>9822789334</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>/maps/api/place/add/json</t>
+  </si>
+  <si>
+    <t>api_Request</t>
+  </si>
+  <si>
+    <t>content_Type</t>
+  </si>
+  <si>
+    <t>POST</t>
   </si>
 </sst>
 </file>
@@ -75,8 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -379,10 +452,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,39 +468,174 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>